<commit_message>
data cleaning more to come
</commit_message>
<xml_diff>
--- a/data/metadata.xlsx
+++ b/data/metadata.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="995" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="995" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Indiana" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="160">
   <si>
     <t>dataset</t>
   </si>
@@ -252,6 +252,51 @@
     <t>total number of registered Naloxone therapy in each county</t>
   </si>
   <si>
+    <t>nrows</t>
+  </si>
+  <si>
+    <t>Local_Unemployment_Statistics-_Labor_force_data_by_county_annual_averages</t>
+  </si>
+  <si>
+    <t>state_fips_code, county_fips_code, county_name, state_abbreviation, year, unemployment_rate</t>
+  </si>
+  <si>
+    <t>state_fips, county_fips, county, state, year, unemployment_rate</t>
+  </si>
+  <si>
+    <t>https://hhs-opioid-codeathon.data.socrata.com/resource/p9fs-ggsh.json</t>
+  </si>
+  <si>
+    <t>not in zip drive, data cleaning needed to adjust state and county info into FIPS code</t>
+  </si>
+  <si>
+    <t>CDC_WONDER_Cause_of_Death___Underlying_Cause__County_</t>
+  </si>
+  <si>
+    <t>year_code, underlying_cause, underlying_cause_1, county, county_code, deaths, population</t>
+  </si>
+  <si>
+    <t>year, primary_cause, primary_cause_code, county, fips, deaths, population</t>
+  </si>
+  <si>
+    <t>https://hhs-opioid-codeathon.data.socrata.com/resource/523d-m6kz.json</t>
+  </si>
+  <si>
+    <t>Medicare_Part_D_Opioid_Prescriber_Summary_File_2013</t>
+  </si>
+  <si>
+    <t>nppes_provider_state, total_claim_count, opioid_claim_count</t>
+  </si>
+  <si>
+    <t>state, medicaire_claims, medicaire_opioid_claims</t>
+  </si>
+  <si>
+    <t>https://hhs-opioid-codeathon.data.socrata.com/resource/vcp5-amce.json</t>
+  </si>
+  <si>
+    <t>no FIPS code, but ZIP code; opioid claim count is blank if &lt; 10</t>
+  </si>
+  <si>
     <t>Dataset</t>
   </si>
   <si>
@@ -303,15 +348,9 @@
     <t>https://hhs-opioid-codeathon.data.socrata.com/resource/azsb-5fi3.json</t>
   </si>
   <si>
-    <t>CDC_WONDER_Cause_of_Death___Underlying_Cause__County_</t>
-  </si>
-  <si>
     <t>Year, Year Code, Underlying Cause of death, Underlying Cause of death Code,County,County Code,Deaths,  Population, Location</t>
   </si>
   <si>
-    <t>https://hhs-opioid-codeathon.data.socrata.com/resource/523d-m6kz.json</t>
-  </si>
-  <si>
     <t>Fatal_Drug_Overdose_Trends__VA_</t>
   </si>
   <si>
@@ -372,21 +411,12 @@
     <t>https://data.medicaid.gov/resource/4qik-skk9.json</t>
   </si>
   <si>
-    <t>Medicare_Part_D_Opioid_Prescriber_Summary_File_2013</t>
-  </si>
-  <si>
     <t>NPPES Provider ZIP Code, NPPES Provide State, Specialty Description, Total Claim Count, Opioid Claim Count, Opioid Prescribing Rate</t>
   </si>
   <si>
     <t>4, 5, 6, 7, 8, 9</t>
   </si>
   <si>
-    <t>https://hhs-opioid-codeathon.data.socrata.com/resource/vcp5-amce.json</t>
-  </si>
-  <si>
-    <t>no FIPS code, but ZIP code; opioid claim count is blank if &lt; 10</t>
-  </si>
-  <si>
     <t>Medicare_Part_D_Opioid_Prescriber_Summary_File_2014</t>
   </si>
   <si>
@@ -421,15 +451,6 @@
   </si>
   <si>
     <t>https://hhs-opioid-codeathon.data.socrata.com/resource/ne85-gheu.json</t>
-  </si>
-  <si>
-    <t>not in zip drive, data cleaning needed to adjust state and county info into FIPS code</t>
-  </si>
-  <si>
-    <t>Local_Unemployment_Statistics-_Labor_force_data_by_county_annual_averages</t>
-  </si>
-  <si>
-    <t>https://hhs-opioid-codeathon.data.socrata.com/resource/p9fs-ggsh.json</t>
   </si>
   <si>
     <t>FHFA_-_Federal_Home_Loan_Bank_Data_-_2009</t>
@@ -577,8 +598,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -613,8 +638,8 @@
   </sheetPr>
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A33" activeCellId="0" sqref="A33"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1086,17 +1111,97 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.5023255813953"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="70.5813953488372"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.5116279069767"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="97.4139534883721"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="66.553488372093"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="63.2558139534884"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.8279069767442"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" s="1" t="n">
+        <v>19314</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>4729</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>1049326</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>90</v>
+      </c>
+    </row>
+  </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -1114,7 +1219,7 @@
   </sheetPr>
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -1129,381 +1234,381 @@
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.35348837209302"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="true" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>81</v>
+    <row r="1" s="2" customFormat="true" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>82</v>
+        <v>97</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>83</v>
+        <v>98</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>84</v>
+        <v>99</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>86</v>
+        <v>100</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>101</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>87</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>88</v>
+        <v>103</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>89</v>
+        <v>104</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>90</v>
+        <v>105</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>91</v>
+        <v>106</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>92</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>94</v>
+        <v>108</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>90</v>
+        <v>105</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>91</v>
+        <v>106</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>96</v>
+        <v>109</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>97</v>
+        <v>110</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>98</v>
+        <v>111</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>99</v>
+        <v>112</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>100</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>102</v>
+        <v>115</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>103</v>
+        <v>116</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>105</v>
+        <v>118</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>106</v>
+        <v>119</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>107</v>
+        <v>120</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>102</v>
+        <v>115</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>103</v>
+        <v>116</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>108</v>
+        <v>121</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>106</v>
+        <v>119</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>109</v>
+        <v>122</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>102</v>
+        <v>115</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>103</v>
+        <v>116</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>111</v>
+        <v>124</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>112</v>
+        <v>125</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>113</v>
+        <v>126</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>114</v>
+        <v>127</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>115</v>
+        <v>128</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>116</v>
+        <v>86</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>117</v>
+        <v>129</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>118</v>
+        <v>130</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>119</v>
+        <v>89</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>120</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>121</v>
+        <v>131</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>117</v>
+        <v>129</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>118</v>
+        <v>130</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>120</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>125</v>
+        <v>135</v>
       </c>
       <c r="B14" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="F14" s="0" t="s">
         <v>126</v>
-      </c>
-      <c r="D14" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="E14" s="0" t="s">
-        <v>128</v>
-      </c>
-      <c r="F14" s="0" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>129</v>
+        <v>139</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="16" s="3" customFormat="true" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="17" s="3" customFormat="true" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>133</v>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="16" s="4" customFormat="true" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="17" s="4" customFormat="true" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="F18" s="3" t="s">
-        <v>137</v>
+      <c r="A18" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="F18" s="4" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>137</v>
+      <c r="A19" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>137</v>
+      <c r="A20" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>137</v>
+      <c r="A21" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>137</v>
+      <c r="A22" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>137</v>
+      <c r="A23" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>137</v>
+      <c r="A24" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="3" t="s">
+      <c r="A25" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="F25" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="F25" s="3" t="s">
-        <v>137</v>
-      </c>
     </row>
     <row r="26" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>133</v>
+      <c r="A26" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="F27" s="3" t="s">
-        <v>148</v>
+      <c r="A27" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="F27" s="4" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>148</v>
+      <c r="A28" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>148</v>
+      <c r="A29" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>148</v>
+      <c r="A30" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="F31" s="3" t="s">
-        <v>148</v>
+      <c r="A31" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>155</v>
       </c>
     </row>
   </sheetData>

</xml_diff>